<commit_message>
Add environment variable configuration and enhance CLI with AI audit capabilities
- Introduced a .env.example file for API key configuration, including OpenAI and optional Anthropic keys.
- Added a new CLI command for AI-powered multi-agent SEO audits, leveraging specialized agents for comprehensive analysis.
- Updated the report command to accept both folder paths and direct summary.json paths for improved usability.
- Enhanced the AppConfig class to load API keys from the environment, supporting multi-agent functionality.
- Revised SEO summaries for clarity and actionable insights in JSON reports.
</commit_message>
<xml_diff>
--- a/reports/example.com/example.com-report.xlsx
+++ b/reports/example.com/example.com-report.xlsx
@@ -477,7 +477,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-11-10T23:56:31.605665Z</t>
+          <t>2025-11-11T01:35:29.265000Z</t>
         </is>
       </c>
     </row>
@@ -492,7 +492,7 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>The website has a missing meta description, which can negatively impact search engine visibility and click-through rates. Addressing this issue will enhance the site's SEO performance.</t>
+          <t>The site has a missing meta description, which can negatively impact its visibility in search results. Addressing this issue will improve click-through rates and overall SEO performance.</t>
         </is>
       </c>
     </row>
@@ -579,9 +579,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="56" customWidth="1" min="1" max="1"/>
+    <col width="58" customWidth="1" min="1" max="1"/>
     <col width="100" customWidth="1" min="2" max="2"/>
-    <col width="64" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -605,7 +605,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>The website has a missing meta description, which can negatively impact search engine visibility and click-through rates. Addressing this issue will enhance the site's SEO performance.</t>
+          <t>The site has a missing meta description, which can negatively impact its visibility in search results. Addressing this issue will improve click-through rates and overall SEO performance.</t>
         </is>
       </c>
       <c r="C2" s="2" t="n"/>
@@ -675,12 +675,12 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>Meta descriptions help improve search engine rankings and attract clicks from users.</t>
+          <t>Meta descriptions help search engines understand page content and influence user clicks.</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>The homepage at https://example.com/ lacks a meta description.</t>
+          <t>The homepage lacks a meta description.</t>
         </is>
       </c>
     </row>
@@ -760,7 +760,7 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Monitor search performance after updates</t>
+          <t>Monitor click-through rates after implementing changes</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
@@ -777,7 +777,7 @@
     <row r="15">
       <c r="A15" s="2" t="inlineStr">
         <is>
-          <t>Educate the team on the importance of meta tags</t>
+          <t>Educate the team on best practices for meta descriptions</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">

</xml_diff>